<commit_message>
formula do CAGR correta
</commit_message>
<xml_diff>
--- a/input/data.xlsx
+++ b/input/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\Documents\GitHub\Analise-IHFA\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB4A8D1-7F42-45AC-8286-0AC6346A5272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F82150A-54ED-46B8-889A-7D6CDDC6E26A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -110,11 +110,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9626DDE1-27E2-4386-8290-0CCC06A08B21}">
   <dimension ref="A1:H164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H43" sqref="H1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1779,7 @@
       <c r="F60" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G60" s="6">
+      <c r="G60" s="4">
         <v>6.3E-3</v>
       </c>
     </row>
@@ -3348,7 +3347,7 @@
         <v>1.0699999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>43313</v>
       </c>
@@ -3371,7 +3370,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>43344</v>
       </c>
@@ -3394,7 +3393,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>43374</v>
       </c>
@@ -3417,7 +3416,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>43405</v>
       </c>
@@ -3440,7 +3439,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>43435</v>
       </c>
@@ -3463,7 +3462,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>43466</v>
       </c>
@@ -3486,7 +3485,7 @@
         <v>2.6100000000000002E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>43497</v>
       </c>
@@ -3509,7 +3508,7 @@
         <v>-2.3E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>43525</v>
       </c>
@@ -3532,7 +3531,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>43556</v>
       </c>
@@ -3555,7 +3554,7 @@
         <v>5.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>43586</v>
       </c>
@@ -3578,7 +3577,7 @@
         <v>9.2999999999999992E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>43617</v>
       </c>
@@ -3600,9 +3599,8 @@
       <c r="G139" s="3">
         <v>1.5100000000000001E-2</v>
       </c>
-      <c r="H139" s="4"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>43647</v>
       </c>
@@ -3624,9 +3622,8 @@
       <c r="G140" s="3">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="H140" s="4"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>43678</v>
       </c>
@@ -3648,9 +3645,8 @@
       <c r="G141" s="3">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="H141" s="4"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>43709</v>
       </c>
@@ -3672,9 +3668,8 @@
       <c r="G142" s="3">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="H142" s="4"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>43739</v>
       </c>
@@ -3696,9 +3691,8 @@
       <c r="G143" s="3">
         <v>1.34E-2</v>
       </c>
-      <c r="H143" s="4"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>43770</v>
       </c>
@@ -3720,7 +3714,6 @@
       <c r="G144" s="3">
         <v>-2.0999999999999999E-3</v>
       </c>
-      <c r="H144" s="4"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
@@ -3744,7 +3737,6 @@
       <c r="G145" s="3">
         <v>2.5399999999999999E-2</v>
       </c>
-      <c r="H145" s="4"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
@@ -3768,7 +3760,6 @@
       <c r="G146" s="1">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="H146" s="4"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
@@ -3792,7 +3783,6 @@
       <c r="G147" s="1">
         <v>-1.5699999999999999E-2</v>
       </c>
-      <c r="H147" s="4"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
@@ -3816,7 +3806,6 @@
       <c r="G148" s="1">
         <v>-6.2399999999999997E-2</v>
       </c>
-      <c r="H148" s="4"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
@@ -3840,7 +3829,6 @@
       <c r="G149" s="1">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="H149" s="4"/>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
@@ -3864,7 +3852,6 @@
       <c r="G150" s="1">
         <v>1.8700000000000001E-2</v>
       </c>
-      <c r="H150" s="4"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
@@ -3888,7 +3875,6 @@
       <c r="G151" s="1">
         <v>1.8100000000000002E-2</v>
       </c>
-      <c r="H151" s="4"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
@@ -3986,6 +3972,7 @@
       <c r="A156" s="2">
         <v>44136</v>
       </c>
+      <c r="H156" s="5"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
@@ -3994,11 +3981,9 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
-      <c r="H158" s="4"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
-      <c r="H159" s="5"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>

</xml_diff>